<commit_message>
changed to saving in excel as a row
</commit_message>
<xml_diff>
--- a/xl_data/image5_0.xlsx
+++ b/xl_data/image5_0.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,130 +424,55 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Type of lecture</t>
+          <t>2nd Module Symposium</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>2nd Module Symposium</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Lecture Title</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
           <t>"Machine Learning Applications in Finance"</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Resource Person Name</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Vivek Kumar</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Designation</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Data Scientist</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Company Name</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Microsoft</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>City,Country</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Mumbai, India</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Course Code/Course Title</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>CSE8856 - Parallel and Distributed Computing</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Date: 9th March, 2024</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Time: 3:00 PM to 5:00 PM</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Mode/Venue</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Mode: Online (MS Teams) - https://shorturl.at/zzFF9</t>
         </is>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Coordinators</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Faculty Coordinators: Dr. Rajesh Sharma, Dr. Smita Patel, Dr. Ravi Kapoor and Dr. Seema Gupta</t>
         </is>

</xml_diff>